<commit_message>
updated competition spreadsheet again
</commit_message>
<xml_diff>
--- a/Docs/Competition.xlsx
+++ b/Docs/Competition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="15315" windowHeight="9915"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="15315" windowHeight="9855"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="122">
   <si>
     <t>Competition</t>
   </si>
@@ -322,6 +322,66 @@
   </si>
   <si>
     <t>Web, iPhone(?)</t>
+  </si>
+  <si>
+    <t>Omnifocus</t>
+  </si>
+  <si>
+    <t>Daytum</t>
+  </si>
+  <si>
+    <t>http://www.daytum.com/</t>
+  </si>
+  <si>
+    <t>lists &amp; statistics</t>
+  </si>
+  <si>
+    <t>Task management</t>
+  </si>
+  <si>
+    <t>http://www.omnigroup.com/products/omnifocus/</t>
+  </si>
+  <si>
+    <t>Mac, iPhone, iPad</t>
+  </si>
+  <si>
+    <t>cloud sync, e-mail integration</t>
+  </si>
+  <si>
+    <t>$80 license</t>
+  </si>
+  <si>
+    <t>ReQall</t>
+  </si>
+  <si>
+    <t>Voice-enabled memory aid</t>
+  </si>
+  <si>
+    <t>http://www.reqall.com/about</t>
+  </si>
+  <si>
+    <t>iPhone, Android, BB</t>
+  </si>
+  <si>
+    <t>connectors for outlook, google cal, evernote</t>
+  </si>
+  <si>
+    <t>Freemium (25/yr)</t>
+  </si>
+  <si>
+    <t>Carbonfin outliner</t>
+  </si>
+  <si>
+    <t>http://carbonfin.com/</t>
+  </si>
+  <si>
+    <t>iPhone, iPad</t>
+  </si>
+  <si>
+    <t>license fee on device</t>
+  </si>
+  <si>
+    <t>sync, collab between users</t>
   </si>
 </sst>
 </file>
@@ -385,8 +445,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J29" totalsRowShown="0">
-  <autoFilter ref="A1:J29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J33" totalsRowShown="0">
+  <autoFilter ref="A1:J33"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Competition"/>
     <tableColumn id="2" name="Category"/>
@@ -690,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +764,7 @@
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1220,6 +1280,89 @@
       </c>
       <c r="J29" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" t="s">
+        <v>110</v>
+      </c>
+      <c r="J30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" t="s">
+        <v>114</v>
+      </c>
+      <c r="I32" t="s">
+        <v>116</v>
+      </c>
+      <c r="J32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" t="s">
+        <v>120</v>
+      </c>
+      <c r="J33" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1238,10 +1381,11 @@
     <hyperlink ref="C14" r:id="rId12"/>
     <hyperlink ref="C28" r:id="rId13"/>
     <hyperlink ref="C29" r:id="rId14"/>
+    <hyperlink ref="C31" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated competition and assumption list docs
</commit_message>
<xml_diff>
--- a/Docs/Competition.xlsx
+++ b/Docs/Competition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="15315" windowHeight="9855"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="14610" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="128">
   <si>
     <t>Competition</t>
   </si>
@@ -382,6 +382,24 @@
   </si>
   <si>
     <t>sync, collab between users</t>
+  </si>
+  <si>
+    <t>Asana</t>
+  </si>
+  <si>
+    <t>http://www.asana.com/</t>
+  </si>
+  <si>
+    <t>Dustin Moskowitz</t>
+  </si>
+  <si>
+    <t>Freemium? (30 free)</t>
+  </si>
+  <si>
+    <t>slick web app - for teams / business</t>
+  </si>
+  <si>
+    <t>Web, mobile</t>
   </si>
 </sst>
 </file>
@@ -445,8 +463,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J33" totalsRowShown="0">
-  <autoFilter ref="A1:J33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J34" totalsRowShown="0">
+  <autoFilter ref="A1:J34"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Competition"/>
     <tableColumn id="2" name="Category"/>
@@ -750,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +782,7 @@
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1363,6 +1381,32 @@
       </c>
       <c r="J33" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" t="s">
+        <v>127</v>
+      </c>
+      <c r="I34" t="s">
+        <v>125</v>
+      </c>
+      <c r="J34" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checked in new vision docs
</commit_message>
<xml_diff>
--- a/Docs/Competition.xlsx
+++ b/Docs/Competition.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="141">
   <si>
     <t>Competition</t>
   </si>
@@ -427,6 +427,18 @@
   </si>
   <si>
     <t>acquired by ebay</t>
+  </si>
+  <si>
+    <t>Any.DO</t>
+  </si>
+  <si>
+    <t>downloaded 0.5M in 30days: http://techcrunch.com/2011/12/12/any-do-android-500000/</t>
+  </si>
+  <si>
+    <t>http://www.any.do/</t>
+  </si>
+  <si>
+    <t>android (iPhone, web coming)</t>
   </si>
 </sst>
 </file>
@@ -490,8 +502,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J36" totalsRowShown="0">
-  <autoFilter ref="A1:J36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J37" totalsRowShown="0">
+  <autoFilter ref="A1:J37"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Competition"/>
     <tableColumn id="2" name="Category"/>
@@ -795,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,6 +1495,26 @@
       </c>
       <c r="J36" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" t="s">
+        <v>140</v>
+      </c>
+      <c r="J37" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>